<commit_message>
for reals this time?
</commit_message>
<xml_diff>
--- a/allmerged.xlsx
+++ b/allmerged.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Classes\biostats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Techy\Documents\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896E4FDA-1639-4F4C-8034-A2B6314E000F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E3B3B62-EC26-4BF9-BB3F-39221CF73A5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2970" yWindow="7785" windowWidth="15555" windowHeight="11490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -22,19 +22,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Pop (thousands)</t>
+    <t>newaggdeaths.country</t>
   </si>
   <si>
-    <t>GDPPC</t>
+    <t>aggdeaths.year</t>
   </si>
   <si>
-    <t>CancerDeaths</t>
+    <t>aggdeaths.AllDeaths</t>
   </si>
   <si>
-    <t>Year</t>
+    <t>X.2</t>
   </si>
   <si>
-    <t>Country</t>
+    <t>Pop (thousands)</t>
   </si>
 </sst>
 </file>
@@ -878,27 +878,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="R121" sqref="R121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2811,8 +2811,9 @@
       <c r="E93" s="1">
         <v>1094</v>
       </c>
-      <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
+      <c r="F93">
+        <v>3676.2060000000001</v>
+      </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
@@ -2830,7 +2831,9 @@
       <c r="E94" s="1">
         <v>1694</v>
       </c>
-      <c r="F94" s="1"/>
+      <c r="F94">
+        <v>4776.8379999999897</v>
+      </c>
       <c r="G94" s="1"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -2849,7 +2852,9 @@
       <c r="E95" s="1">
         <v>2220</v>
       </c>
-      <c r="F95" s="1"/>
+      <c r="F95">
+        <v>24299.168000000001</v>
+      </c>
       <c r="G95" s="1"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -2868,7 +2873,9 @@
       <c r="E96" s="1">
         <v>1176</v>
       </c>
-      <c r="F96" s="1"/>
+      <c r="F96">
+        <v>69784.087</v>
+      </c>
       <c r="G96" s="1"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -2887,8 +2894,9 @@
       <c r="E97" s="1">
         <v>1975</v>
       </c>
-      <c r="F97" s="1"/>
-      <c r="G97" s="1"/>
+      <c r="F97">
+        <v>37133.86</v>
+      </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
@@ -2906,7 +2914,9 @@
       <c r="E98" s="1">
         <v>3696</v>
       </c>
-      <c r="F98" s="1"/>
+      <c r="F98">
+        <v>38458.642</v>
+      </c>
       <c r="G98" s="1"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -2925,8 +2935,9 @@
       <c r="E99" s="1">
         <v>2716</v>
       </c>
-      <c r="F99" s="1"/>
-      <c r="G99" s="1"/>
+      <c r="F99">
+        <v>9929.1759999999904</v>
+      </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
@@ -2944,7 +2955,9 @@
       <c r="E100" s="1">
         <v>11639</v>
       </c>
-      <c r="F100" s="1"/>
+      <c r="F100">
+        <v>10091.322</v>
+      </c>
       <c r="G100" s="1"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -2963,8 +2976,9 @@
       <c r="E101" s="1">
         <v>6106</v>
       </c>
-      <c r="F101" s="1"/>
-      <c r="G101" s="1"/>
+      <c r="F101">
+        <v>3263.1729999999902</v>
+      </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102">
@@ -2982,7 +2996,9 @@
       <c r="E102" s="1">
         <v>11721</v>
       </c>
-      <c r="F102" s="1"/>
+      <c r="F102">
+        <v>3567.6909999999898</v>
+      </c>
       <c r="G102" s="1"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3001,8 +3017,9 @@
       <c r="E103" s="1">
         <v>2196</v>
       </c>
-      <c r="F103" s="1"/>
-      <c r="G103" s="1"/>
+      <c r="F103">
+        <v>23071.258000000002</v>
+      </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104">
@@ -3020,7 +3037,9 @@
       <c r="E104" s="1">
         <v>1640</v>
       </c>
-      <c r="F104" s="1"/>
+      <c r="F104">
+        <v>22964.746999999901</v>
+      </c>
       <c r="G104" s="1"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3039,7 +3058,9 @@
       <c r="E105" s="1">
         <v>2713</v>
       </c>
-      <c r="F105" s="1"/>
+      <c r="F105">
+        <v>148227.470999999</v>
+      </c>
       <c r="G105" s="1"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3058,8 +3079,9 @@
       <c r="E106" s="1">
         <v>2524</v>
       </c>
-      <c r="F106" s="1"/>
-      <c r="G106" s="1"/>
+      <c r="F106">
+        <v>41.874000000000002</v>
+      </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107">
@@ -3077,7 +3099,9 @@
       <c r="E107" s="1">
         <v>6987</v>
       </c>
-      <c r="F107" s="1"/>
+      <c r="F107">
+        <v>42.076999999999899</v>
+      </c>
       <c r="G107" s="1"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -3096,8 +3120,9 @@
       <c r="E108" s="1">
         <v>4072</v>
       </c>
-      <c r="F108" s="1"/>
-      <c r="G108" s="1"/>
+      <c r="F108">
+        <v>7.29199999999999</v>
+      </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109">
@@ -3115,7 +3140,9 @@
       <c r="E109" s="1">
         <v>10583</v>
       </c>
-      <c r="F109" s="1"/>
+      <c r="F109">
+        <v>9.8680000000000003</v>
+      </c>
       <c r="G109" s="1"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -3134,7 +3161,9 @@
       <c r="E110" s="1">
         <v>4199</v>
       </c>
-      <c r="F110" s="1"/>
+      <c r="F110">
+        <v>146.87100000000001</v>
+      </c>
       <c r="G110" s="1"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -3153,8 +3182,9 @@
       <c r="E111" s="1">
         <v>39407</v>
       </c>
-      <c r="F111" s="1"/>
-      <c r="G111" s="1"/>
+      <c r="F111">
+        <v>25.925000000000001</v>
+      </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112">
@@ -3172,7 +3202,9 @@
       <c r="E112" s="1">
         <v>69338</v>
       </c>
-      <c r="F112" s="1"/>
+      <c r="F112">
+        <v>29.324000000000002</v>
+      </c>
       <c r="G112" s="1"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -3191,6 +3223,9 @@
       <c r="E113">
         <v>759</v>
       </c>
+      <c r="F113">
+        <v>104.926</v>
+      </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114">
@@ -3208,7 +3243,9 @@
       <c r="E114" s="1">
         <v>2922</v>
       </c>
-      <c r="F114" s="1"/>
+      <c r="F114">
+        <v>69.772000000000006</v>
+      </c>
       <c r="G114" s="1"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -3227,7 +3264,9 @@
       <c r="E115" s="1">
         <v>6858</v>
       </c>
-      <c r="F115" s="1"/>
+      <c r="F115">
+        <v>2705.5369999999898</v>
+      </c>
       <c r="G115" s="1"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -3246,7 +3285,9 @@
       <c r="E116" s="1">
         <v>25265</v>
       </c>
-      <c r="F116" s="1"/>
+      <c r="F116">
+        <v>3525.9639999999899</v>
+      </c>
       <c r="G116" s="1"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -3265,7 +3306,9 @@
       <c r="E117" s="1">
         <v>28372</v>
       </c>
-      <c r="F117" s="1"/>
+      <c r="F117">
+        <v>4265.6930000000002</v>
+      </c>
       <c r="G117" s="1"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -3284,7 +3327,9 @@
       <c r="E118" s="1">
         <v>46592</v>
       </c>
-      <c r="F118" s="1"/>
+      <c r="F118">
+        <v>5131.17</v>
+      </c>
       <c r="G118" s="1"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -3303,7 +3348,9 @@
       <c r="E119" s="1">
         <v>10683</v>
       </c>
-      <c r="F119" s="1"/>
+      <c r="F119">
+        <v>1991.126</v>
+      </c>
       <c r="G119" s="1"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -3322,7 +3369,9 @@
       <c r="E120" s="1">
         <v>3741</v>
       </c>
-      <c r="F120" s="1"/>
+      <c r="F120">
+        <v>41435.760999999897</v>
+      </c>
       <c r="G120" s="1"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -3341,8 +3390,9 @@
       <c r="E121" s="1">
         <v>4643</v>
       </c>
-      <c r="F121" s="1"/>
-      <c r="G121" s="1"/>
+      <c r="F121">
+        <v>38733.866000000002</v>
+      </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122">
@@ -3360,7 +3410,9 @@
       <c r="E122" s="1">
         <v>15366</v>
       </c>
-      <c r="F122" s="1"/>
+      <c r="F122">
+        <v>39787.413</v>
+      </c>
       <c r="G122" s="1"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -3379,7 +3431,9 @@
       <c r="E123" s="1">
         <v>3221</v>
       </c>
-      <c r="F123" s="1"/>
+      <c r="F123">
+        <v>368.63600000000002</v>
+      </c>
       <c r="G123" s="1"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -3398,7 +3452,9 @@
       <c r="E124" s="1">
         <v>29915</v>
       </c>
-      <c r="F124" s="1"/>
+      <c r="F124">
+        <v>8836.4210000000003</v>
+      </c>
       <c r="G124" s="1"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -3417,8 +3473,9 @@
       <c r="E125" s="1">
         <v>1382</v>
       </c>
-      <c r="F125" s="1"/>
-      <c r="G125" s="1"/>
+      <c r="F125">
+        <v>135274.08300000001</v>
+      </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126">
@@ -3436,7 +3493,9 @@
       <c r="E126" s="1">
         <v>4794</v>
       </c>
-      <c r="F126" s="1"/>
+      <c r="F126">
+        <v>162019.889</v>
+      </c>
       <c r="G126" s="1"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -3455,6 +3514,9 @@
       <c r="E127">
         <v>944</v>
       </c>
+      <c r="F127">
+        <v>10648.633</v>
+      </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128">
@@ -3472,6 +3534,9 @@
       <c r="E128">
         <v>211</v>
       </c>
+      <c r="F128">
+        <v>4537.82</v>
+      </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129">
@@ -3489,6 +3554,9 @@
       <c r="E129">
         <v>337</v>
       </c>
+      <c r="F129">
+        <v>5764.8059999999896</v>
+      </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130">
@@ -3506,6 +3574,9 @@
       <c r="E130">
         <v>775</v>
       </c>
+      <c r="F130">
+        <v>52026.900999999903</v>
+      </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131">
@@ -3523,8 +3594,9 @@
       <c r="E131" s="1">
         <v>6282</v>
       </c>
-      <c r="F131" s="1"/>
-      <c r="G131" s="1"/>
+      <c r="F131">
+        <v>1170.296</v>
+      </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132">
@@ -3542,7 +3614,9 @@
       <c r="E132" s="1">
         <v>4235</v>
       </c>
-      <c r="F132" s="1"/>
+      <c r="F132">
+        <v>1254.2</v>
+      </c>
       <c r="G132" s="1"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -3561,6 +3635,9 @@
       <c r="E133">
         <v>520</v>
       </c>
+      <c r="F133">
+        <v>4207.8410000000003</v>
+      </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134">
@@ -3578,8 +3655,9 @@
       <c r="E134" s="1">
         <v>6142</v>
       </c>
-      <c r="F134" s="1"/>
-      <c r="G134" s="1"/>
+      <c r="F134">
+        <v>9.9740000000000002</v>
+      </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135">
@@ -3597,7 +3675,9 @@
       <c r="E135" s="1">
         <v>12425</v>
       </c>
-      <c r="F135" s="1"/>
+      <c r="F135">
+        <v>16.221</v>
+      </c>
       <c r="G135" s="1"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -3616,6 +3696,9 @@
       <c r="E136">
         <v>770</v>
       </c>
+      <c r="F136">
+        <v>3112.9229999999902</v>
+      </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137">
@@ -3633,7 +3716,9 @@
       <c r="E137" s="1">
         <v>2615</v>
       </c>
-      <c r="F137" s="1"/>
+      <c r="F137">
+        <v>3086.81</v>
+      </c>
       <c r="G137" s="1"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -3652,7 +3737,9 @@
       <c r="E138" s="1">
         <v>4056</v>
       </c>
-      <c r="F138" s="1"/>
+      <c r="F138">
+        <v>2948.029</v>
+      </c>
       <c r="G138" s="1"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -3671,6 +3758,9 @@
       <c r="E139">
         <v>990</v>
       </c>
+      <c r="F139">
+        <v>50903.783000000003</v>
+      </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140">
@@ -3688,7 +3778,9 @@
       <c r="E140" s="1">
         <v>2834</v>
       </c>
-      <c r="F140" s="1"/>
+      <c r="F140">
+        <v>206.96199999999899</v>
+      </c>
       <c r="G140" s="1"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -3707,8 +3799,9 @@
       <c r="E141" s="1">
         <v>18017</v>
       </c>
-      <c r="F141" s="1"/>
-      <c r="G141" s="1"/>
+      <c r="F141">
+        <v>240499.821999999</v>
+      </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142">
@@ -3726,7 +3819,9 @@
       <c r="E142" s="1">
         <v>28758</v>
       </c>
-      <c r="F142" s="1"/>
+      <c r="F142">
+        <v>265163.74099999899</v>
+      </c>
       <c r="G142" s="1"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -3745,8 +3840,9 @@
       <c r="E143" s="1">
         <v>1735</v>
       </c>
-      <c r="F143" s="1"/>
-      <c r="G143" s="1"/>
+      <c r="F143">
+        <v>3011.5189999999898</v>
+      </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144">
@@ -3764,7 +3860,9 @@
       <c r="E144" s="1">
         <v>6609</v>
       </c>
-      <c r="F144" s="1"/>
+      <c r="F144">
+        <v>3224.2750000000001</v>
+      </c>
       <c r="G144" s="1"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -3783,6 +3881,9 @@
       <c r="E145">
         <v>589</v>
       </c>
+      <c r="F145">
+        <v>22791.032999999901</v>
+      </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146">
@@ -3800,8 +3901,9 @@
       <c r="E146" s="1">
         <v>3396</v>
       </c>
-      <c r="F146" s="1"/>
-      <c r="G146" s="1"/>
+      <c r="F146">
+        <v>13.951000000000001</v>
+      </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147">
@@ -3819,7 +3921,9 @@
       <c r="E147" s="1">
         <v>21114</v>
       </c>
-      <c r="F147" s="1"/>
+      <c r="F147">
+        <v>19.306999999999899</v>
+      </c>
       <c r="G147" s="1"/>
     </row>
   </sheetData>
@@ -3828,4 +3932,207 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007216D139ABABCC4AB82616842869C9C5" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8d175aa560902c16ab589888d8ce740">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e9414cb6-4861-4f4d-bf3a-58843a58901b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0854d198982e5d666b236a43d6a097ee" ns3:_="">
+    <xsd:import namespace="e9414cb6-4861-4f4d-bf3a-58843a58901b"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e9414cb6-4861-4f4d-bf3a-58843a58901b" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49378144-D773-4AB2-AEE1-E83E9ACD9879}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e9414cb6-4861-4f4d-bf3a-58843a58901b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5092D69-D50C-4188-BAA2-40BE8369A567}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{118B4A44-D6F2-4E63-96E0-E18527C226C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e9414cb6-4861-4f4d-bf3a-58843a58901b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>